<commit_message>
Refs #2749 assigning benefit group to census_employees
</commit_message>
<xml_diff>
--- a/spec/test_data/spreadsheet_templates/DCHL Employee Census.xlsx
+++ b/spec/test_data/spreadsheet_templates/DCHL Employee Census.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="300" windowWidth="28540" windowHeight="14480" tabRatio="488"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="488"/>
   </bookViews>
   <sheets>
     <sheet name="Employee Census" sheetId="6" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
   <si>
     <t>Last Name</t>
   </si>
@@ -316,6 +316,12 @@
   </si>
   <si>
     <t>female</t>
+  </si>
+  <si>
+    <t>plan_year</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Plan Year (Optional)</t>
   </si>
 </sst>
 </file>
@@ -1377,11 +1383,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N313"/>
+  <dimension ref="A1:O313"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1398,12 +1404,13 @@
     <col min="10" max="10" width="12.6640625" style="27" customWidth="1"/>
     <col min="11" max="12" width="11.33203125" style="15" customWidth="1"/>
     <col min="13" max="13" width="12.6640625" style="27" customWidth="1"/>
-    <col min="14" max="14" width="21.1640625" style="17" customWidth="1"/>
-    <col min="15" max="19" width="9.1640625" style="14" customWidth="1"/>
+    <col min="14" max="14" width="13.5" style="17" customWidth="1"/>
+    <col min="15" max="15" width="16" style="14" customWidth="1"/>
+    <col min="16" max="19" width="9.1640625" style="14" customWidth="1"/>
     <col min="20" max="16384" width="9.1640625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="20" customFormat="1" ht="31.25" customHeight="1">
+    <row r="1" spans="1:15" s="20" customFormat="1" ht="31.25" customHeight="1">
       <c r="A1" s="21" t="s">
         <v>4</v>
       </c>
@@ -1425,7 +1432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" customFormat="1" ht="31.25" customHeight="1">
+    <row r="2" spans="1:15" customFormat="1" ht="31.25" customHeight="1">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1468,8 +1475,11 @@
       <c r="N2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" ht="56">
+      <c r="O2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="56">
       <c r="A3" s="29" t="s">
         <v>5</v>
       </c>
@@ -1512,8 +1522,11 @@
       <c r="N3" s="31" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="O3" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
@@ -1555,8 +1568,11 @@
         <f>+IF(ISBLANK($A4),"","Main Benefit Group")</f>
         <v>Main Benefit Group</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="O4" s="9">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>37</v>
       </c>
@@ -1594,8 +1610,11 @@
         <f t="shared" ref="N5:N68" si="0">+IF(ISBLANK($A5),"","Main Benefit Group")</f>
         <v>Main Benefit Group</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="O5" s="9">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A6" s="2">
         <v>14567</v>
       </c>
@@ -1635,8 +1654,11 @@
         <f t="shared" si="0"/>
         <v>Main Benefit Group</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="O6" s="9">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A7" s="2">
         <v>14568</v>
       </c>
@@ -1674,8 +1696,11 @@
         <f t="shared" si="0"/>
         <v>Main Benefit Group</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="O7" s="9">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A8" s="2">
         <v>14569</v>
       </c>
@@ -1713,8 +1738,11 @@
         <f t="shared" si="0"/>
         <v>Main Benefit Group</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="O8" s="9">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1733,7 +1761,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="10" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1752,7 +1780,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="11" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1771,7 +1799,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="12" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1790,7 +1818,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="13" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1809,7 +1837,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="14" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1828,7 +1856,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="15" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1847,7 +1875,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="16" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>

</xml_diff>

<commit_message>
add upload employee roster to empty roster view
</commit_message>
<xml_diff>
--- a/spec/test_data/spreadsheet_templates/DCHL Employee Census.xlsx
+++ b/spec/test_data/spreadsheet_templates/DCHL Employee Census.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="488"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14740" tabRatio="488"/>
   </bookViews>
   <sheets>
     <sheet name="Employee Census" sheetId="6" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Last Name</t>
   </si>
@@ -229,93 +229,6 @@
   </si>
   <si>
     <t>employee_relationship</t>
-  </si>
-  <si>
-    <t>abc123</t>
-  </si>
-  <si>
-    <t>Employee</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>sr</t>
-  </si>
-  <si>
-    <t>abc124</t>
-  </si>
-  <si>
-    <t>111-33-3333</t>
-  </si>
-  <si>
-    <t>111-44-4444</t>
-  </si>
-  <si>
-    <t>111-11-1111</t>
-  </si>
-  <si>
-    <t>111-22-2222</t>
-  </si>
-  <si>
-    <t>111-55-5555</t>
-  </si>
-  <si>
-    <t>panther</t>
-  </si>
-  <si>
-    <t>pink</t>
-  </si>
-  <si>
-    <t>runner</t>
-  </si>
-  <si>
-    <t>road</t>
-  </si>
-  <si>
-    <t>coyote</t>
-  </si>
-  <si>
-    <t>wiley</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>bunny</t>
-  </si>
-  <si>
-    <t>bugs</t>
-  </si>
-  <si>
-    <t>fudd</t>
-  </si>
-  <si>
-    <t>elmer</t>
-  </si>
-  <si>
-    <t>bbunny@warnerbros.com</t>
-  </si>
-  <si>
-    <t>efudd@warnerbros.com</t>
-  </si>
-  <si>
-    <t>wcoyote@warnerbros.com</t>
-  </si>
-  <si>
-    <t>rr@warnerbros.com</t>
-  </si>
-  <si>
-    <t>pink@warnerbros.com</t>
-  </si>
-  <si>
-    <t>female</t>
   </si>
   <si>
     <t>plan_year</t>
@@ -1387,7 +1300,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A4:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1476,7 +1389,7 @@
         <v>17</v>
       </c>
       <c r="O2" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" ht="56">
@@ -1523,221 +1436,100 @@
         <v>25</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" s="5">
-        <v>23673</v>
-      </c>
-      <c r="J4" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="6">
-        <v>40695</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="6"/>
       <c r="L4" s="6"/>
-      <c r="M4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4" s="8" t="str">
-        <f>+IF(ISBLANK($A4),"","Main Benefit Group")</f>
-        <v>Main Benefit Group</v>
-      </c>
+      <c r="M4" s="3"/>
+      <c r="N4" s="8"/>
       <c r="O4" s="9">
         <v>2015</v>
       </c>
     </row>
     <row r="5" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="5">
-        <v>15593</v>
-      </c>
-      <c r="J5" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="K5" s="6">
-        <v>41411</v>
-      </c>
+      <c r="G5" s="35"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="6"/>
       <c r="L5" s="6"/>
-      <c r="M5" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="N5" s="8" t="str">
-        <f t="shared" ref="N5:N68" si="0">+IF(ISBLANK($A5),"","Main Benefit Group")</f>
-        <v>Main Benefit Group</v>
-      </c>
+      <c r="M5" s="25"/>
+      <c r="N5" s="8"/>
       <c r="O5" s="9">
         <v>2015</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A6" s="2">
-        <v>14567</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>49</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="5">
-        <v>14701</v>
-      </c>
-      <c r="J6" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="6">
-        <v>41487</v>
-      </c>
+      <c r="G6" s="34"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="6"/>
       <c r="L6" s="6"/>
-      <c r="M6" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="N6" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Main Benefit Group</v>
-      </c>
+      <c r="M6" s="24"/>
+      <c r="N6" s="8"/>
       <c r="O6" s="9">
         <v>2015</v>
       </c>
     </row>
     <row r="7" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A7" s="2">
-        <v>14568</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="5">
-        <v>17695</v>
-      </c>
-      <c r="J7" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="K7" s="6">
-        <v>41488</v>
-      </c>
+      <c r="G7" s="34"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="6"/>
       <c r="L7" s="6"/>
-      <c r="M7" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="N7" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Main Benefit Group</v>
-      </c>
+      <c r="M7" s="24"/>
+      <c r="N7" s="8"/>
       <c r="O7" s="9">
         <v>2014</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="2">
-        <v>14569</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="5">
-        <v>15525</v>
-      </c>
-      <c r="J8" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="6">
-        <v>42208</v>
-      </c>
+      <c r="G8" s="34"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="6"/>
       <c r="L8" s="6"/>
-      <c r="M8" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="N8" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Main Benefit Group</v>
-      </c>
+      <c r="M8" s="24"/>
+      <c r="N8" s="8"/>
       <c r="O8" s="9">
         <v>2014</v>
       </c>
@@ -1757,7 +1549,7 @@
       <c r="L9" s="6"/>
       <c r="M9" s="24"/>
       <c r="N9" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="N5:N68" si="0">+IF(ISBLANK($A9),"","Main Benefit Group")</f>
         <v/>
       </c>
     </row>
@@ -7539,13 +7331,6 @@
     </dataValidation>
     <dataValidation operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:L1048576"/>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="G4" r:id="rId1"/>
-    <hyperlink ref="G5" r:id="rId2"/>
-    <hyperlink ref="G6" r:id="rId3"/>
-    <hyperlink ref="G7" r:id="rId4"/>
-    <hyperlink ref="G8" r:id="rId5"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
Refs #2999 Added address fields to the template and upload code
</commit_message>
<xml_diff>
--- a/spec/test_data/spreadsheet_templates/DCHL Employee Census.xlsx
+++ b/spec/test_data/spreadsheet_templates/DCHL Employee Census.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="488"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16260" tabRatio="488"/>
   </bookViews>
   <sheets>
     <sheet name="Employee Census" sheetId="6" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>Last Name</t>
   </si>
@@ -249,72 +249,6 @@
     <t>sr</t>
   </si>
   <si>
-    <t>abc124</t>
-  </si>
-  <si>
-    <t>111-33-3333</t>
-  </si>
-  <si>
-    <t>111-44-4444</t>
-  </si>
-  <si>
-    <t>111-11-1111</t>
-  </si>
-  <si>
-    <t>111-22-2222</t>
-  </si>
-  <si>
-    <t>111-55-5555</t>
-  </si>
-  <si>
-    <t>panther</t>
-  </si>
-  <si>
-    <t>pink</t>
-  </si>
-  <si>
-    <t>runner</t>
-  </si>
-  <si>
-    <t>road</t>
-  </si>
-  <si>
-    <t>coyote</t>
-  </si>
-  <si>
-    <t>wiley</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>bunny</t>
-  </si>
-  <si>
-    <t>bugs</t>
-  </si>
-  <si>
-    <t>fudd</t>
-  </si>
-  <si>
-    <t>elmer</t>
-  </si>
-  <si>
-    <t>bbunny@warnerbros.com</t>
-  </si>
-  <si>
-    <t>efudd@warnerbros.com</t>
-  </si>
-  <si>
-    <t>wcoyote@warnerbros.com</t>
-  </si>
-  <si>
-    <t>rr@warnerbros.com</t>
-  </si>
-  <si>
-    <t>pink@warnerbros.com</t>
-  </si>
-  <si>
     <t>female</t>
   </si>
   <si>
@@ -322,6 +256,72 @@
   </si>
   <si>
     <t xml:space="preserve"> Plan Year (Optional)</t>
+  </si>
+  <si>
+    <t>111@gmail.com</t>
+  </si>
+  <si>
+    <t>Child</t>
+  </si>
+  <si>
+    <t>runner1</t>
+  </si>
+  <si>
+    <t>road1</t>
+  </si>
+  <si>
+    <t>panther1</t>
+  </si>
+  <si>
+    <t>pink1</t>
+  </si>
+  <si>
+    <t>address_1</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>100 NY Avenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Washington </t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>kind</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>Address Kind(Optional)</t>
+  </si>
+  <si>
+    <t>Address Line 1(Optional)</t>
+  </si>
+  <si>
+    <t>City(Optional)</t>
+  </si>
+  <si>
+    <t>State(Optional)</t>
+  </si>
+  <si>
+    <t>Zip(Optional)</t>
+  </si>
+  <si>
+    <t>111111110</t>
+  </si>
+  <si>
+    <t>111229990</t>
   </si>
 </sst>
 </file>
@@ -678,7 +678,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -823,8 +823,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="76">
+  <cellStyleXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -902,6 +917,9 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -997,11 +1015,11 @@
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="73" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="76">
+  <cellStyles count="79">
     <cellStyle name="20% - Accent1 2" xfId="4"/>
     <cellStyle name="20% - Accent2 2" xfId="5"/>
     <cellStyle name="20% - Accent3 2" xfId="6"/>
@@ -1044,6 +1062,9 @@
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Good 2" xfId="36"/>
     <cellStyle name="Heading 1 2" xfId="37"/>
     <cellStyle name="Heading 2 2" xfId="38"/>
@@ -1383,11 +1404,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O313"/>
+  <dimension ref="A1:T310"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1405,12 +1426,14 @@
     <col min="11" max="12" width="11.33203125" style="15" customWidth="1"/>
     <col min="13" max="13" width="12.6640625" style="27" customWidth="1"/>
     <col min="14" max="14" width="13.5" style="17" customWidth="1"/>
-    <col min="15" max="15" width="16" style="14" customWidth="1"/>
-    <col min="16" max="19" width="9.1640625" style="14" customWidth="1"/>
-    <col min="20" max="16384" width="9.1640625" style="14"/>
+    <col min="15" max="16" width="18.5" style="14" customWidth="1"/>
+    <col min="17" max="17" width="17.83203125" style="14" customWidth="1"/>
+    <col min="18" max="18" width="20.1640625" style="14" customWidth="1"/>
+    <col min="19" max="20" width="9.1640625" style="14" customWidth="1"/>
+    <col min="21" max="16384" width="9.1640625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="20" customFormat="1" ht="31.25" customHeight="1">
+    <row r="1" spans="1:20" s="20" customFormat="1" ht="31.25" customHeight="1">
       <c r="A1" s="21" t="s">
         <v>4</v>
       </c>
@@ -1432,7 +1455,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" customFormat="1" ht="31.25" customHeight="1">
+    <row r="2" spans="1:20" customFormat="1" ht="31.25" customHeight="1">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1476,10 +1499,25 @@
         <v>17</v>
       </c>
       <c r="O2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="56">
+        <v>38</v>
+      </c>
+      <c r="P2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S2" t="s">
+        <v>48</v>
+      </c>
+      <c r="T2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" s="1" customFormat="1" ht="56">
       <c r="A3" s="29" t="s">
         <v>5</v>
       </c>
@@ -1522,11 +1560,26 @@
       <c r="N3" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="O3" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q3" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="R3" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="S3" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="T3" s="35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
@@ -1534,10 +1587,10 @@
         <v>32</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>35</v>
@@ -1546,13 +1599,13 @@
         <v>36</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="I4" s="5">
-        <v>23673</v>
+        <v>14699</v>
       </c>
       <c r="J4" s="24" t="s">
         <v>33</v>
@@ -1565,184 +1618,116 @@
         <v>34</v>
       </c>
       <c r="N4" s="8" t="str">
-        <f>+IF(ISBLANK($A4),"","Main Benefit Group")</f>
-        <v>Main Benefit Group</v>
+        <f>+IF(ISBLANK($A4),"","bf1")</f>
+        <v>bf1</v>
       </c>
       <c r="O4" s="9">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
+        <v>2016</v>
+      </c>
+      <c r="P4" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="S4" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="T4" s="9">
+        <v>20001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="35" t="s">
-        <v>57</v>
-      </c>
+      <c r="G5" s="34"/>
       <c r="H5" s="7" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="I5" s="5">
-        <v>15593</v>
+        <v>36249</v>
       </c>
       <c r="J5" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="K5" s="6">
-        <v>41411</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="K5" s="6"/>
       <c r="L5" s="6"/>
-      <c r="M5" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="N5" s="8" t="str">
-        <f t="shared" ref="N5:N68" si="0">+IF(ISBLANK($A5),"","Main Benefit Group")</f>
-        <v>Main Benefit Group</v>
-      </c>
-      <c r="O5" s="9">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A6" s="2">
-        <v>14567</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>49</v>
-      </c>
+      <c r="M5" s="25"/>
+      <c r="N5" s="8"/>
+    </row>
+    <row r="6" spans="1:20" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="5">
-        <v>14701</v>
-      </c>
-      <c r="J6" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="6">
-        <v>41487</v>
-      </c>
+      <c r="G6" s="24"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="6"/>
       <c r="L6" s="6"/>
-      <c r="M6" s="24" t="s">
-        <v>34</v>
-      </c>
+      <c r="M6" s="24"/>
       <c r="N6" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Main Benefit Group</v>
-      </c>
-      <c r="O6" s="9">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A7" s="2">
-        <v>14568</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>51</v>
-      </c>
+        <f t="shared" ref="N6:N65" si="0">+IF(ISBLANK($A6),"","Main Benefit Group")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:20" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="5">
-        <v>17695</v>
-      </c>
-      <c r="J7" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="K7" s="6">
-        <v>41488</v>
-      </c>
+      <c r="G7" s="24"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="6"/>
       <c r="L7" s="6"/>
-      <c r="M7" s="24" t="s">
-        <v>34</v>
-      </c>
+      <c r="M7" s="24"/>
       <c r="N7" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>Main Benefit Group</v>
-      </c>
-      <c r="O7" s="9">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="2">
-        <v>14569</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>53</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:20" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="5">
-        <v>15525</v>
-      </c>
-      <c r="J8" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="6">
-        <v>42208</v>
-      </c>
+      <c r="G8" s="24"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="6"/>
       <c r="L8" s="6"/>
-      <c r="M8" s="24" t="s">
-        <v>34</v>
-      </c>
+      <c r="M8" s="24"/>
       <c r="N8" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>Main Benefit Group</v>
-      </c>
-      <c r="O8" s="9">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:20" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1761,7 +1746,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="10" spans="1:20" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1780,7 +1765,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="11" spans="1:20" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1799,7 +1784,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="12" spans="1:20" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1818,7 +1803,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="13" spans="1:20" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1837,7 +1822,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="14" spans="1:20" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1856,7 +1841,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="15" spans="1:20" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1875,7 +1860,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="16" spans="1:20" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -2840,7 +2825,7 @@
       <c r="L66" s="6"/>
       <c r="M66" s="24"/>
       <c r="N66" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="N66:N129" si="1">+IF(ISBLANK($A66),"","Main Benefit Group")</f>
         <v/>
       </c>
     </row>
@@ -2859,7 +2844,7 @@
       <c r="L67" s="6"/>
       <c r="M67" s="24"/>
       <c r="N67" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2878,7 +2863,7 @@
       <c r="L68" s="6"/>
       <c r="M68" s="24"/>
       <c r="N68" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2897,7 +2882,7 @@
       <c r="L69" s="6"/>
       <c r="M69" s="24"/>
       <c r="N69" s="8" t="str">
-        <f t="shared" ref="N69:N132" si="1">+IF(ISBLANK($A69),"","Main Benefit Group")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -4056,7 +4041,7 @@
       <c r="L130" s="6"/>
       <c r="M130" s="24"/>
       <c r="N130" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="N130:N193" si="2">+IF(ISBLANK($A130),"","Main Benefit Group")</f>
         <v/>
       </c>
     </row>
@@ -4075,7 +4060,7 @@
       <c r="L131" s="6"/>
       <c r="M131" s="24"/>
       <c r="N131" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -4094,7 +4079,7 @@
       <c r="L132" s="6"/>
       <c r="M132" s="24"/>
       <c r="N132" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -4113,7 +4098,7 @@
       <c r="L133" s="6"/>
       <c r="M133" s="24"/>
       <c r="N133" s="8" t="str">
-        <f t="shared" ref="N133:N196" si="2">+IF(ISBLANK($A133),"","Main Benefit Group")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -5272,7 +5257,7 @@
       <c r="L194" s="6"/>
       <c r="M194" s="24"/>
       <c r="N194" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="N194:N257" si="3">+IF(ISBLANK($A194),"","Main Benefit Group")</f>
         <v/>
       </c>
     </row>
@@ -5291,7 +5276,7 @@
       <c r="L195" s="6"/>
       <c r="M195" s="24"/>
       <c r="N195" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -5310,7 +5295,7 @@
       <c r="L196" s="6"/>
       <c r="M196" s="24"/>
       <c r="N196" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -5329,7 +5314,7 @@
       <c r="L197" s="6"/>
       <c r="M197" s="24"/>
       <c r="N197" s="8" t="str">
-        <f t="shared" ref="N197:N260" si="3">+IF(ISBLANK($A197),"","Main Benefit Group")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -6302,58 +6287,58 @@
         <v/>
       </c>
     </row>
-    <row r="249" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A249" s="2"/>
-      <c r="B249" s="3"/>
-      <c r="C249" s="3"/>
-      <c r="D249" s="3"/>
-      <c r="E249" s="4"/>
-      <c r="F249" s="4"/>
-      <c r="G249" s="24"/>
-      <c r="H249" s="7"/>
-      <c r="I249" s="5"/>
-      <c r="J249" s="24"/>
-      <c r="K249" s="6"/>
-      <c r="L249" s="6"/>
-      <c r="M249" s="24"/>
+    <row r="249" spans="1:14" ht="15" customHeight="1">
+      <c r="A249" s="10"/>
+      <c r="B249" s="10"/>
+      <c r="C249" s="10"/>
+      <c r="D249" s="10"/>
+      <c r="E249" s="10"/>
+      <c r="F249" s="10"/>
+      <c r="G249" s="26"/>
+      <c r="H249" s="12"/>
+      <c r="I249" s="11"/>
+      <c r="J249" s="26"/>
+      <c r="K249" s="11"/>
+      <c r="L249" s="11"/>
+      <c r="M249" s="26"/>
       <c r="N249" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="250" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A250" s="2"/>
-      <c r="B250" s="3"/>
-      <c r="C250" s="3"/>
-      <c r="D250" s="3"/>
-      <c r="E250" s="4"/>
-      <c r="F250" s="4"/>
-      <c r="G250" s="24"/>
-      <c r="H250" s="7"/>
-      <c r="I250" s="5"/>
-      <c r="J250" s="24"/>
-      <c r="K250" s="6"/>
-      <c r="L250" s="6"/>
-      <c r="M250" s="24"/>
+    <row r="250" spans="1:14" ht="15" customHeight="1">
+      <c r="A250" s="10"/>
+      <c r="B250" s="10"/>
+      <c r="C250" s="10"/>
+      <c r="D250" s="10"/>
+      <c r="E250" s="10"/>
+      <c r="F250" s="10"/>
+      <c r="G250" s="26"/>
+      <c r="H250" s="12"/>
+      <c r="I250" s="11"/>
+      <c r="J250" s="26"/>
+      <c r="K250" s="11"/>
+      <c r="L250" s="11"/>
+      <c r="M250" s="26"/>
       <c r="N250" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="251" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A251" s="2"/>
-      <c r="B251" s="3"/>
-      <c r="C251" s="3"/>
-      <c r="D251" s="3"/>
-      <c r="E251" s="4"/>
-      <c r="F251" s="4"/>
-      <c r="G251" s="24"/>
-      <c r="H251" s="7"/>
-      <c r="I251" s="5"/>
-      <c r="J251" s="24"/>
-      <c r="K251" s="6"/>
-      <c r="L251" s="6"/>
-      <c r="M251" s="24"/>
+    <row r="251" spans="1:14" ht="15" customHeight="1">
+      <c r="A251" s="10"/>
+      <c r="B251" s="10"/>
+      <c r="C251" s="10"/>
+      <c r="D251" s="10"/>
+      <c r="E251" s="10"/>
+      <c r="F251" s="10"/>
+      <c r="G251" s="26"/>
+      <c r="H251" s="12"/>
+      <c r="I251" s="11"/>
+      <c r="J251" s="26"/>
+      <c r="K251" s="11"/>
+      <c r="L251" s="11"/>
+      <c r="M251" s="26"/>
       <c r="N251" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -6488,7 +6473,7 @@
       <c r="L258" s="11"/>
       <c r="M258" s="26"/>
       <c r="N258" s="8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="N258:N310" si="4">+IF(ISBLANK($A258),"","Main Benefit Group")</f>
         <v/>
       </c>
     </row>
@@ -6507,7 +6492,7 @@
       <c r="L259" s="11"/>
       <c r="M259" s="26"/>
       <c r="N259" s="8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -6526,7 +6511,7 @@
       <c r="L260" s="11"/>
       <c r="M260" s="26"/>
       <c r="N260" s="8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -6545,7 +6530,7 @@
       <c r="L261" s="11"/>
       <c r="M261" s="26"/>
       <c r="N261" s="8" t="str">
-        <f t="shared" ref="N261:N313" si="4">+IF(ISBLANK($A261),"","Main Benefit Group")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -7443,88 +7428,31 @@
       </c>
     </row>
     <row r="309" spans="1:14" ht="15" customHeight="1">
-      <c r="A309" s="10"/>
-      <c r="B309" s="10"/>
-      <c r="C309" s="10"/>
-      <c r="D309" s="10"/>
-      <c r="E309" s="10"/>
-      <c r="F309" s="10"/>
-      <c r="G309" s="26"/>
-      <c r="H309" s="12"/>
-      <c r="I309" s="11"/>
-      <c r="J309" s="26"/>
-      <c r="K309" s="11"/>
-      <c r="L309" s="11"/>
-      <c r="M309" s="26"/>
       <c r="N309" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="310" spans="1:14" ht="15" customHeight="1">
-      <c r="A310" s="10"/>
-      <c r="B310" s="10"/>
-      <c r="C310" s="10"/>
-      <c r="D310" s="10"/>
-      <c r="E310" s="10"/>
-      <c r="F310" s="10"/>
-      <c r="G310" s="26"/>
-      <c r="H310" s="12"/>
-      <c r="I310" s="11"/>
-      <c r="J310" s="26"/>
-      <c r="K310" s="11"/>
-      <c r="L310" s="11"/>
-      <c r="M310" s="26"/>
       <c r="N310" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="311" spans="1:14" ht="15" customHeight="1">
-      <c r="A311" s="10"/>
-      <c r="B311" s="10"/>
-      <c r="C311" s="10"/>
-      <c r="D311" s="10"/>
-      <c r="E311" s="10"/>
-      <c r="F311" s="10"/>
-      <c r="G311" s="26"/>
-      <c r="H311" s="12"/>
-      <c r="I311" s="11"/>
-      <c r="J311" s="26"/>
-      <c r="K311" s="11"/>
-      <c r="L311" s="11"/>
-      <c r="M311" s="26"/>
-      <c r="N311" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="312" spans="1:14" ht="15" customHeight="1">
-      <c r="N312" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="313" spans="1:14" ht="15" customHeight="1">
-      <c r="N313" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F311 IR4:IR311 SN4:SN311 ACJ4:ACJ311 AMF4:AMF311 AWB4:AWB311 BFX4:BFX311 BPT4:BPT311 BZP4:BZP311 CJL4:CJL311 CTH4:CTH311 DDD4:DDD311 DMZ4:DMZ311 DWV4:DWV311 EGR4:EGR311 EQN4:EQN311 FAJ4:FAJ311 FKF4:FKF311 FUB4:FUB311 GDX4:GDX311 GNT4:GNT311 GXP4:GXP311 HHL4:HHL311 HRH4:HRH311 IBD4:IBD311 IKZ4:IKZ311 IUV4:IUV311 JER4:JER311 JON4:JON311 JYJ4:JYJ311 KIF4:KIF311 KSB4:KSB311 LBX4:LBX311 LLT4:LLT311 LVP4:LVP311 MFL4:MFL311 MPH4:MPH311 MZD4:MZD311 NIZ4:NIZ311 NSV4:NSV311 OCR4:OCR311 OMN4:OMN311 OWJ4:OWJ311 PGF4:PGF311 PQB4:PQB311 PZX4:PZX311 QJT4:QJT311 QTP4:QTP311 RDL4:RDL311 RNH4:RNH311 RXD4:RXD311 SGZ4:SGZ311 SQV4:SQV311 TAR4:TAR311 TKN4:TKN311 TUJ4:TUJ311 UEF4:UEF311 UOB4:UOB311 UXX4:UXX311 VHT4:VHT311 VRP4:VRP311 WBL4:WBL311 WLH4:WLH311 WVD4:WVD311">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B305:B308 WVA4:WVA308 WLE4:WLE308 WBI4:WBI308 VRM4:VRM308 VHQ4:VHQ308 UXU4:UXU308 UNY4:UNY308 UEC4:UEC308 TUG4:TUG308 TKK4:TKK308 TAO4:TAO308 SQS4:SQS308 SGW4:SGW308 RXA4:RXA308 RNE4:RNE308 RDI4:RDI308 QTM4:QTM308 QJQ4:QJQ308 PZU4:PZU308 PPY4:PPY308 PGC4:PGC308 OWG4:OWG308 OMK4:OMK308 OCO4:OCO308 NSS4:NSS308 NIW4:NIW308 MZA4:MZA308 MPE4:MPE308 MFI4:MFI308 LVM4:LVM308 LLQ4:LLQ308 LBU4:LBU308 KRY4:KRY308 KIC4:KIC308 JYG4:JYG308 JOK4:JOK308 JEO4:JEO308 IUS4:IUS308 IKW4:IKW308 IBA4:IBA308 HRE4:HRE308 HHI4:HHI308 GXM4:GXM308 GNQ4:GNQ308 GDU4:GDU308 FTY4:FTY308 FKC4:FKC308 FAG4:FAG308 EQK4:EQK308 EGO4:EGO308 DWS4:DWS308 DMW4:DMW308 DDA4:DDA308 CTE4:CTE308 CJI4:CJI308 BZM4:BZM308 BPQ4:BPQ308 BFU4:BFU308 AVY4:AVY308 AMC4:AMC308 ACG4:ACG308 SK4:SK308 IO4:IO308">
+      <formula1>EERelationships</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVE4:WVE308 WLI4:WLI308 WBM4:WBM308 VRQ4:VRQ308 VHU4:VHU308 UXY4:UXY308 UOC4:UOC308 UEG4:UEG308 TUK4:TUK308 TKO4:TKO308 TAS4:TAS308 SQW4:SQW308 SHA4:SHA308 RXE4:RXE308 RNI4:RNI308 RDM4:RDM308 QTQ4:QTQ308 QJU4:QJU308 PZY4:PZY308 PQC4:PQC308 PGG4:PGG308 OWK4:OWK308 OMO4:OMO308 OCS4:OCS308 NSW4:NSW308 NJA4:NJA308 MZE4:MZE308 MPI4:MPI308 MFM4:MFM308 LVQ4:LVQ308 LLU4:LLU308 LBY4:LBY308 KSC4:KSC308 KIG4:KIG308 JYK4:JYK308 JOO4:JOO308 JES4:JES308 IUW4:IUW308 ILA4:ILA308 IBE4:IBE308 HRI4:HRI308 HHM4:HHM308 GXQ4:GXQ308 GNU4:GNU308 GDY4:GDY308 FUC4:FUC308 FKG4:FKG308 FAK4:FAK308 EQO4:EQO308 EGS4:EGS308 DWW4:DWW308 DNA4:DNA308 DDE4:DDE308 CTI4:CTI308 CJM4:CJM308 BZQ4:BZQ308 BPU4:BPU308 BFY4:BFY308 AWC4:AWC308 AMG4:AMG308 ACK4:ACK308 SO4:SO308 IS4:IS308 F4:F308">
       <formula1>Suffix</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="IW4:IX311 SS4:ST311 ACO4:ACP311 AMK4:AML311 AWG4:AWH311 BGC4:BGD311 BPY4:BPZ311 BZU4:BZV311 CJQ4:CJR311 CTM4:CTN311 DDI4:DDJ311 DNE4:DNF311 DXA4:DXB311 EGW4:EGX311 EQS4:EQT311 FAO4:FAP311 FKK4:FKL311 FUG4:FUH311 GEC4:GED311 GNY4:GNZ311 GXU4:GXV311 HHQ4:HHR311 HRM4:HRN311 IBI4:IBJ311 ILE4:ILF311 IVA4:IVB311 JEW4:JEX311 JOS4:JOT311 JYO4:JYP311 KIK4:KIL311 KSG4:KSH311 LCC4:LCD311 LLY4:LLZ311 LVU4:LVV311 MFQ4:MFR311 MPM4:MPN311 MZI4:MZJ311 NJE4:NJF311 NTA4:NTB311 OCW4:OCX311 OMS4:OMT311 OWO4:OWP311 PGK4:PGL311 PQG4:PQH311 QAC4:QAD311 QJY4:QJZ311 QTU4:QTV311 RDQ4:RDR311 RNM4:RNN311 RXI4:RXJ311 SHE4:SHF311 SRA4:SRB311 TAW4:TAX311 TKS4:TKT311 TUO4:TUP311 UEK4:UEL311 UOG4:UOH311 UYC4:UYD311 VHY4:VHZ311 VRU4:VRV311 WBQ4:WBR311 WLM4:WLN311 WVI4:WVJ311">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="WVJ4:WVK308 WLN4:WLO308 WBR4:WBS308 VRV4:VRW308 VHZ4:VIA308 UYD4:UYE308 UOH4:UOI308 UEL4:UEM308 TUP4:TUQ308 TKT4:TKU308 TAX4:TAY308 SRB4:SRC308 SHF4:SHG308 RXJ4:RXK308 RNN4:RNO308 RDR4:RDS308 QTV4:QTW308 QJZ4:QKA308 QAD4:QAE308 PQH4:PQI308 PGL4:PGM308 OWP4:OWQ308 OMT4:OMU308 OCX4:OCY308 NTB4:NTC308 NJF4:NJG308 MZJ4:MZK308 MPN4:MPO308 MFR4:MFS308 LVV4:LVW308 LLZ4:LMA308 LCD4:LCE308 KSH4:KSI308 KIL4:KIM308 JYP4:JYQ308 JOT4:JOU308 JEX4:JEY308 IVB4:IVC308 ILF4:ILG308 IBJ4:IBK308 HRN4:HRO308 HHR4:HHS308 GXV4:GXW308 GNZ4:GOA308 GED4:GEE308 FUH4:FUI308 FKL4:FKM308 FAP4:FAQ308 EQT4:EQU308 EGX4:EGY308 DXB4:DXC308 DNF4:DNG308 DDJ4:DDK308 CTN4:CTO308 CJR4:CJS308 BZV4:BZW308 BPZ4:BQA308 BGD4:BGE308 AWH4:AWI308 AML4:AMM308 ACP4:ACQ308 ST4:SU308 IX4:IY308">
       <formula1>Status</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="IN4:IN311 SJ4:SJ311 ACF4:ACF311 AMB4:AMB311 AVX4:AVX311 BFT4:BFT311 BPP4:BPP311 BZL4:BZL311 CJH4:CJH311 CTD4:CTD311 DCZ4:DCZ311 DMV4:DMV311 DWR4:DWR311 EGN4:EGN311 EQJ4:EQJ311 FAF4:FAF311 FKB4:FKB311 FTX4:FTX311 GDT4:GDT311 GNP4:GNP311 GXL4:GXL311 HHH4:HHH311 HRD4:HRD311 IAZ4:IAZ311 IKV4:IKV311 IUR4:IUR311 JEN4:JEN311 JOJ4:JOJ311 JYF4:JYF311 KIB4:KIB311 KRX4:KRX311 LBT4:LBT311 LLP4:LLP311 LVL4:LVL311 MFH4:MFH311 MPD4:MPD311 MYZ4:MYZ311 NIV4:NIV311 NSR4:NSR311 OCN4:OCN311 OMJ4:OMJ311 OWF4:OWF311 PGB4:PGB311 PPX4:PPX311 PZT4:PZT311 QJP4:QJP311 QTL4:QTL311 RDH4:RDH311 RND4:RND311 RWZ4:RWZ311 SGV4:SGV311 SQR4:SQR311 TAN4:TAN311 TKJ4:TKJ311 TUF4:TUF311 UEB4:UEB311 UNX4:UNX311 UXT4:UXT311 VHP4:VHP311 VRL4:VRL311 WBH4:WBH311 WLD4:WLD311 WUZ4:WUZ311 B308:B311">
-      <formula1>EERelationships</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B307">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B304">
       <formula1>"Employee,Spouse,Domestic Partner,Child,Disabled Child"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576">
@@ -7541,10 +7469,6 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1"/>
-    <hyperlink ref="G5" r:id="rId2"/>
-    <hyperlink ref="G6" r:id="rId3"/>
-    <hyperlink ref="G7" r:id="rId4"/>
-    <hyperlink ref="G8" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>